<commit_message>
Font updated to Arial 10
</commit_message>
<xml_diff>
--- a/002594.SZ.xlsx
+++ b/002594.SZ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1.Finance\Anaylsen\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A8CFBF-64C5-4A60-BB16-CEABCCA62582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374DED04-02AB-453E-8D6C-A85843A2D2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="4680" windowWidth="38175" windowHeight="15240" xr2:uid="{70FF95B8-6525-4A9C-B2C0-3718F646D6B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21060" xr2:uid="{70FF95B8-6525-4A9C-B2C0-3718F646D6B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0;\(#,##0\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,12 +84,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -98,6 +96,20 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -121,11 +133,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -464,75 +477,77 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="2" customWidth="1"/>
+    <col min="2" max="8" width="9.140625" style="2"/>
+    <col min="9" max="9" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="2">
         <v>372</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="3">
         <v>2910.0592360000001</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="3">
         <f>+I2*I3</f>
         <v>1082542.0357920001</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H6" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H7" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="3">
         <f>+I4-I5+I6</f>
         <v>1082542.0357920001</v>
       </c>

</xml_diff>